<commit_message>
updated stability charts problem
</commit_message>
<xml_diff>
--- a/docs/unit2/03_limiteq1/swedish.xlsx
+++ b/docs/unit2/03_limiteq1/swedish.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC759761-EFEB-8448-AA30-BE3688B39A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="780" windowWidth="22740" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -180,9 +181,6 @@
     <t xml:space="preserve">F = </t>
   </si>
   <si>
-    <t>Brigham Young University - CE En 544</t>
-  </si>
-  <si>
     <r>
       <t>a</t>
     </r>
@@ -198,11 +196,14 @@
       <t xml:space="preserve"> [rad]</t>
     </r>
   </si>
+  <si>
+    <t>Brigham Young University - CE 544</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -373,13 +374,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>88900</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -387,6 +388,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1031"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -401,7 +405,7 @@
               <a:avLst/>
             </a:prstGeom>
             <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+              <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -410,7 +414,7 @@
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -432,13 +436,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>342900</xdr:colOff>
           <xdr:row>36</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>657225</xdr:colOff>
+          <xdr:colOff>660400</xdr:colOff>
           <xdr:row>50</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -446,6 +450,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1027"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -460,7 +467,7 @@
               <a:avLst/>
             </a:prstGeom>
             <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+              <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -469,7 +476,7 @@
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -497,11 +504,17 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>113456</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="5" name="Rectangle 4"/>
+            <xdr:cNvPr id="5" name="Rectangle 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -668,7 +681,7 @@
                     <m:f>
                       <m:fPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1600" i="0">
+                          <a:rPr lang="en-US" sz="1600" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -681,7 +694,7 @@
                             <m:subHide m:val="on"/>
                             <m:supHide m:val="on"/>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1600" i="0">
+                              <a:rPr lang="en-US" sz="1600" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
@@ -718,7 +731,7 @@
                             <m:subHide m:val="on"/>
                             <m:supHide m:val="on"/>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1600" i="0">
+                              <a:rPr lang="en-US" sz="1600" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
@@ -756,7 +769,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="Rectangle 4"/>
@@ -920,9 +933,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -960,9 +973,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -997,7 +1010,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1032,7 +1045,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1205,35 +1218,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="8.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="2" customWidth="1"/>
-    <col min="7" max="10" width="9.140625" style="2"/>
-    <col min="11" max="11" width="11.28515625" style="2" customWidth="1"/>
+    <col min="2" max="4" width="9.1640625" style="2"/>
+    <col min="5" max="5" width="8.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="2" customWidth="1"/>
+    <col min="7" max="10" width="9.1640625" style="2"/>
+    <col min="11" max="11" width="11.33203125" style="2" customWidth="1"/>
     <col min="12" max="12" width="11" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
@@ -1245,7 +1258,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1256,7 +1269,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1267,7 +1280,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1278,7 +1291,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -1301,7 +1314,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>7</v>
@@ -1316,7 +1329,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>1</v>
       </c>
@@ -1338,7 +1351,7 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>2</v>
       </c>
@@ -1362,7 +1375,7 @@
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>3</v>
       </c>
@@ -1386,7 +1399,7 @@
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>4</v>
       </c>
@@ -1412,7 +1425,7 @@
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>5</v>
       </c>
@@ -1438,7 +1451,7 @@
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>6</v>
       </c>
@@ -1464,7 +1477,7 @@
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>7</v>
       </c>
@@ -1488,7 +1501,7 @@
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>8</v>
       </c>
@@ -1512,7 +1525,7 @@
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>9</v>
       </c>
@@ -1534,7 +1547,7 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>10</v>
       </c>
@@ -1556,7 +1569,7 @@
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>11</v>
       </c>
@@ -1578,22 +1591,22 @@
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="K23" s="11" t="s">
         <v>14</v>
       </c>
       <c r="L23" s="9"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
     </row>
   </sheetData>
@@ -1611,13 +1624,13 @@
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>304800</xdr:colOff>
                 <xdr:row>25</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:rowOff>88900</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>11</xdr:col>
                 <xdr:colOff>38100</xdr:colOff>
                 <xdr:row>35</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>25400</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1636,13 +1649,13 @@
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>342900</xdr:colOff>
                 <xdr:row>36</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:rowOff>177800</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>657225</xdr:colOff>
+                <xdr:colOff>660400</xdr:colOff>
                 <xdr:row>50</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>25400</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1657,26 +1670,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>